<commit_message>
script and CTVA updates
</commit_message>
<xml_diff>
--- a/CTVA.xlsx
+++ b/CTVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corey\github\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD9A6FB-A04C-40BB-A910-CCDE5E6F2090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011A9F2-EA97-4E54-B774-EC5EF08B3441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18500" yWindow="1450" windowWidth="17730" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11020" yWindow="1050" windowWidth="10870" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={78645751-A3DB-42EC-85EC-483A93FFA059}</author>
+    <author>tc={375CBB10-88FA-4C95-9648-2D91B5F24642}</author>
+    <author>tc={02882332-C43D-4BEF-8906-113891A429C3}</author>
+    <author>tc={D1B4856E-EEDD-4FC9-8960-BC9C3D9A5207}</author>
+    <author>tc={037E3C55-28FE-4865-BE0F-2C6C8F0BF827}</author>
+    <author>tc={E09695EF-B9E4-4E00-ADD7-68048C7205B8}</author>
+  </authors>
+  <commentList>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{78645751-A3DB-42EC-85EC-483A93FFA059}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Price gains were driven by the continued execution on the company's price for value strategy with strong execution across all regions in response to cost inflation, and recovery of higher input costs. </t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{375CBB10-88FA-4C95-9648-2D91B5F24642}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Price gains were driven by continued execution on the company's price for value strategy, strong demand for new technology and strong execution in response to cost inflation led by EMEA, partially offset by challenging market dynamics in Latin America and North America </t>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="2" shapeId="0" xr:uid="{02882332-C43D-4BEF-8906-113891A429C3}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The increase in volume was driven by continued penetration of new products and gains in all regions, partially offset by reduced corn acres in North America and supply constraints in North America canola </t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="3" shapeId="0" xr:uid="{D1B4856E-EEDD-4FC9-8960-BC9C3D9A5207}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Volume declines were driven by strategic product exits, crop protection channel inventory destocking, delayed farmer purchases, lower corn planted area in EMEA, reduced summer corn planted area and lower expected Safrinha corn planted area in Brazil, and the Russia Exit, partially offset by increased corn acres in North America. </t>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="4" shapeId="0" xr:uid="{037E3C55-28FE-4865-BE0F-2C6C8F0BF827}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The portfolio impact was driven by a divestiture in Asia Pacific. </t>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="5" shapeId="0" xr:uid="{E09695EF-B9E4-4E00-ADD7-68048C7205B8}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The portfolio and other impact was driven by the biologicals acquisitions and the sale of seeds already under production in Russia when the decision to exit the country was made and that the company was contractually required to purchase. </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="279">
   <si>
     <t>P</t>
   </si>
@@ -772,9 +835,6 @@
     <t>Worldwide Sales</t>
   </si>
   <si>
-    <t>Net Sales Change YoY</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -794,6 +854,96 @@
   </si>
   <si>
     <t>Portfolio/Other</t>
+  </si>
+  <si>
+    <t>COGS</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>SG&amp;A</t>
+  </si>
+  <si>
+    <t>Amotization of Intangibles</t>
+  </si>
+  <si>
+    <t>Restructuring and Asset Related Charges</t>
+  </si>
+  <si>
+    <t>Other Income</t>
+  </si>
+  <si>
+    <t>Interest Expense</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Worldwide Sales Change YoY</t>
+  </si>
+  <si>
+    <t>Seed Sales</t>
+  </si>
+  <si>
+    <t>Seed operating EBITDA</t>
+  </si>
+  <si>
+    <t>Corn YoY Change</t>
+  </si>
+  <si>
+    <t>Soybean YoY Change</t>
+  </si>
+  <si>
+    <t>Other oilseeds YoY Change</t>
+  </si>
+  <si>
+    <t>Other seed YoY Change</t>
+  </si>
+  <si>
+    <t>Corn YoY Percentage Change</t>
+  </si>
+  <si>
+    <t>Soybean YoY Percentage Change</t>
+  </si>
+  <si>
+    <t>Other oilseeds Percentage YoY Change</t>
+  </si>
+  <si>
+    <t>Other seed Percentage YoY Change</t>
+  </si>
+  <si>
+    <t>Crop Protection Sales</t>
+  </si>
+  <si>
+    <t>Crop Protection EBITDA</t>
+  </si>
+  <si>
+    <t>Herbicides YoY Change</t>
+  </si>
+  <si>
+    <t>Herbicides YoY Percentage Change</t>
+  </si>
+  <si>
+    <t>Insecticides YoY Change</t>
+  </si>
+  <si>
+    <t>Insecticides YoY Percentage Change</t>
+  </si>
+  <si>
+    <t>Fungicides YoY Change</t>
+  </si>
+  <si>
+    <t>Fungicides Percentage YoY Change</t>
+  </si>
+  <si>
+    <t>Other Crop Protection YoY Change</t>
+  </si>
+  <si>
+    <t>Other Crop Prot. Percentage YoY Change</t>
+  </si>
+  <si>
+    <t>Worldwide Seed Sales Change YoY</t>
   </si>
 </sst>
 </file>
@@ -801,8 +951,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -877,7 +1027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -887,20 +1037,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -969,6 +1118,61 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798CE17C-5C00-6A48-C3E1-FB7E73D908C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2787650" y="44450"/>
+          <a:ext cx="12700" cy="9258300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1061,7 +1265,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1154,7 +1358,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1333,7 +1537,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1380,6 +1584,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Corey Christner" id="{96B94962-3352-4CD0-9600-990C74CCBDE4}" userId="32906c935fa0eb4f" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1643,210 +1853,237 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C15" dT="2025-01-23T04:07:32.21" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{78645751-A3DB-42EC-85EC-483A93FFA059}">
+    <text xml:space="preserve">Price gains were driven by the continued execution on the company's price for value strategy with strong execution across all regions in response to cost inflation, and recovery of higher input costs. </text>
+  </threadedComment>
+  <threadedComment ref="D15" dT="2025-01-23T04:13:56.18" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{375CBB10-88FA-4C95-9648-2D91B5F24642}">
+    <text xml:space="preserve">Price gains were driven by continued execution on the company's price for value strategy, strong demand for new technology and strong execution in response to cost inflation led by EMEA, partially offset by challenging market dynamics in Latin America and North America </text>
+  </threadedComment>
+  <threadedComment ref="C16" dT="2025-01-23T04:08:07.88" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{02882332-C43D-4BEF-8906-113891A429C3}">
+    <text xml:space="preserve">The increase in volume was driven by continued penetration of new products and gains in all regions, partially offset by reduced corn acres in North America and supply constraints in North America canola </text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2025-01-23T04:13:35.80" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{D1B4856E-EEDD-4FC9-8960-BC9C3D9A5207}">
+    <text xml:space="preserve">Volume declines were driven by strategic product exits, crop protection channel inventory destocking, delayed farmer purchases, lower corn planted area in EMEA, reduced summer corn planted area and lower expected Safrinha corn planted area in Brazil, and the Russia Exit, partially offset by increased corn acres in North America. </text>
+  </threadedComment>
+  <threadedComment ref="C18" dT="2025-01-23T04:12:35.38" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{037E3C55-28FE-4865-BE0F-2C6C8F0BF827}">
+    <text xml:space="preserve">The portfolio impact was driven by a divestiture in Asia Pacific. </text>
+  </threadedComment>
+  <threadedComment ref="D18" dT="2025-01-23T04:16:52.12" personId="{96B94962-3352-4CD0-9600-990C74CCBDE4}" id="{E09695EF-B9E4-4E00-ADD7-68048C7205B8}">
+    <text xml:space="preserve">The portfolio and other impact was driven by the biologicals acquisitions and the sale of seeds already under production in Russia when the decision to exit the country was made and that the company was contractually required to purchase. </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O63"/>
+  <dimension ref="B2:O60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="14" width="8.7265625" style="8"/>
-    <col min="15" max="15" width="9.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="8"/>
+    <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2">
         <v>62.51</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="9">
         <v>45679</v>
       </c>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="9" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="11">
         <v>687.29300000000001</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="9" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="10">
         <f>+N3*N2</f>
         <v>42962.685429999998</v>
       </c>
     </row>
     <row r="5" spans="2:15">
-      <c r="M5" s="8" t="s">
+      <c r="M5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:15">
-      <c r="M7" s="8" t="s">
+      <c r="M7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="8">
+      <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="33" spans="2:9">
-      <c r="B33" s="8">
+      <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="14.5" customHeight="1">
-      <c r="B34" s="8">
+      <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
     </row>
     <row r="35" spans="2:9">
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
+      <c r="C35" s="8"/>
+      <c r="D35" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
     </row>
     <row r="36" spans="2:9">
-      <c r="B36" s="8">
+      <c r="B36">
         <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>210</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37" spans="2:9">
-      <c r="B37" s="8">
+      <c r="B37">
         <v>5</v>
       </c>
       <c r="C37" t="s">
         <v>211</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="2:9">
-      <c r="B38" s="8">
+      <c r="B38">
         <v>6</v>
       </c>
       <c r="C38" t="s">
@@ -1854,7 +2091,7 @@
       </c>
     </row>
     <row r="39" spans="2:9">
-      <c r="B39" s="8">
+      <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
@@ -1862,12 +2099,12 @@
       </c>
     </row>
     <row r="40" spans="2:9">
-      <c r="D40" s="8" t="s">
+      <c r="D40" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="41" spans="2:9">
-      <c r="B41" s="8">
+      <c r="B41">
         <v>8</v>
       </c>
       <c r="C41" t="s">
@@ -1875,7 +2112,7 @@
       </c>
     </row>
     <row r="42" spans="2:9">
-      <c r="B42" s="8">
+      <c r="B42">
         <v>9</v>
       </c>
       <c r="C42" t="s">
@@ -1883,25 +2120,25 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="D43" s="8" t="s">
+      <c r="D43" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="44" spans="2:9">
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="45" spans="2:9">
-      <c r="B45" s="8">
+      <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="46" spans="2:9">
-      <c r="B46" s="8">
+      <c r="B46">
         <v>2</v>
       </c>
       <c r="C46" t="s">
@@ -1909,15 +2146,15 @@
       </c>
     </row>
     <row r="47" spans="2:9">
-      <c r="B47" s="8">
+      <c r="B47">
         <v>3</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="48" spans="2:9">
-      <c r="B48" s="8">
+      <c r="B48">
         <v>4</v>
       </c>
       <c r="C48" t="s">
@@ -1925,7 +2162,7 @@
       </c>
     </row>
     <row r="49" spans="2:3">
-      <c r="B49" s="8">
+      <c r="B49">
         <v>5</v>
       </c>
       <c r="C49" t="s">
@@ -1933,7 +2170,7 @@
       </c>
     </row>
     <row r="50" spans="2:3">
-      <c r="B50" s="8">
+      <c r="B50">
         <v>6</v>
       </c>
       <c r="C50" t="s">
@@ -1941,7 +2178,7 @@
       </c>
     </row>
     <row r="51" spans="2:3">
-      <c r="B51" s="8">
+      <c r="B51">
         <v>7</v>
       </c>
       <c r="C51" t="s">
@@ -1949,7 +2186,7 @@
       </c>
     </row>
     <row r="52" spans="2:3">
-      <c r="B52" s="8">
+      <c r="B52">
         <v>8</v>
       </c>
       <c r="C52" t="s">
@@ -1957,7 +2194,7 @@
       </c>
     </row>
     <row r="53" spans="2:3">
-      <c r="B53" s="8">
+      <c r="B53">
         <v>9</v>
       </c>
       <c r="C53" t="s">
@@ -1965,7 +2202,7 @@
       </c>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="8">
+      <c r="B54">
         <v>10</v>
       </c>
       <c r="C54" t="s">
@@ -1973,7 +2210,7 @@
       </c>
     </row>
     <row r="55" spans="2:3">
-      <c r="B55" s="8">
+      <c r="B55">
         <v>11</v>
       </c>
       <c r="C55" t="s">
@@ -1981,7 +2218,7 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="8">
+      <c r="B56">
         <v>12</v>
       </c>
       <c r="C56" t="s">
@@ -1989,13 +2226,12 @@
       </c>
     </row>
     <row r="57" spans="2:3">
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C57"/>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="8">
+      <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
@@ -2003,7 +2239,7 @@
       </c>
     </row>
     <row r="59" spans="2:3">
-      <c r="B59" s="8">
+      <c r="B59">
         <v>2</v>
       </c>
       <c r="C59" t="s">
@@ -2011,26 +2247,17 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="8">
+      <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="2:3">
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="2:3">
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="2:3">
-      <c r="C63"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" location="Seed!A1" display="Seed" xr:uid="{C1A0C046-A824-456B-B91A-9178EAE9DEA2}"/>
-    <hyperlink ref="B4" location="CropProtection!A1" display="Crop Protection" xr:uid="{7A53ABF8-5E98-4AB9-8AAF-925DF00DC83D}"/>
+    <hyperlink ref="C3" location="Seed!A1" display="Seed" xr:uid="{C1A0C046-A824-456B-B91A-9178EAE9DEA2}"/>
+    <hyperlink ref="C4" location="CropProtection!A1" display="Crop Protection" xr:uid="{7A53ABF8-5E98-4AB9-8AAF-925DF00DC83D}"/>
     <hyperlink ref="B6" location="IP!A1" display="Intellectual Prop" xr:uid="{D1A5B7E0-37AA-4E55-BD15-9E7C55050CA6}"/>
     <hyperlink ref="B8" location="Litigation!A1" display="Litigation" xr:uid="{9D4E5E58-94DA-4F28-9CC4-6000F227C15C}"/>
   </hyperlinks>
@@ -2040,17 +2267,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B5B72-37FF-40EE-B2C0-12ADFCFD6369}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B5B72-37FF-40EE-B2C0-12ADFCFD6369}">
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2087,140 +2313,556 @@
     <row r="4" spans="1:5" s="3" customFormat="1">
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="5" spans="1:5" s="3" customFormat="1">
+      <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="14">
-        <f>+SUM(B7:B10)</f>
+      <c r="B5" s="12">
+        <f>+SUM(B6:B9)</f>
         <v>15655</v>
       </c>
-      <c r="C6" s="14">
-        <f t="shared" ref="C6:D6" si="0">+SUM(C7:C10)</f>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:D5" si="0">+SUM(C6:C9)</f>
         <v>17455</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>17226</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="10">
+        <v>7536</v>
+      </c>
+      <c r="C6" s="10">
+        <v>8294</v>
+      </c>
+      <c r="D6" s="10">
+        <v>8590</v>
+      </c>
+    </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="15">
-        <v>7536</v>
-      </c>
-      <c r="C7" s="15">
-        <v>8294</v>
-      </c>
-      <c r="D7" s="15">
-        <v>8590</v>
+        <v>238</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3123</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3256</v>
+      </c>
+      <c r="D7" s="10">
+        <v>3367</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>238</v>
-      </c>
-      <c r="B8" s="15">
-        <v>3123</v>
-      </c>
-      <c r="C8" s="15">
-        <v>3256</v>
-      </c>
-      <c r="D8" s="15">
-        <v>3367</v>
+        <v>239</v>
+      </c>
+      <c r="B8" s="10">
+        <v>3545</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4445</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3906</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B9" s="15">
-        <v>3545</v>
-      </c>
-      <c r="C9" s="15">
-        <v>4445</v>
-      </c>
-      <c r="D9" s="15">
-        <v>3906</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
         <v>240</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B9" s="10">
         <v>1451</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C9" s="10">
         <v>1460</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D9" s="10">
         <v>1363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1">
+      <c r="A11" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>242</v>
       </c>
+      <c r="C12" s="12">
+        <f>C5-B5</f>
+        <v>1800</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D5-C5</f>
+        <v>-229</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C13" s="14">
-        <f>C6-B6</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="3" customFormat="1">
+      <c r="C13" s="13">
+        <f>(C5-B5)/B5</f>
+        <v>0.11497923985946981</v>
+      </c>
+      <c r="D13" s="13">
+        <f>(D5-C5)/C5</f>
+        <v>-1.3119450014322544E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="16">
-        <f>(C6-B6)/B6</f>
-        <v>0.11497923985946981</v>
-      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="17" customFormat="1">
-      <c r="A16" s="17" t="s">
+      <c r="C15" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="18">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="17" customFormat="1">
-      <c r="A17" s="17" t="s">
+      <c r="C16" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="14">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>247</v>
       </c>
-      <c r="C17" s="18">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="17" customFormat="1">
-      <c r="A18" s="17" t="s">
+      <c r="C17" s="14">
+        <v>-0.03</v>
+      </c>
+      <c r="D17" s="14">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>248</v>
       </c>
-      <c r="C18" s="18">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="17" customFormat="1">
-      <c r="A19" s="17" t="s">
+      <c r="C18" s="14">
+        <v>-0.01</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="16" customFormat="1">
+      <c r="A20" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="16">
+        <v>8402</v>
+      </c>
+      <c r="C20" s="16">
+        <v>8979</v>
+      </c>
+      <c r="D20" s="16">
+        <v>9472</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="16" customFormat="1">
+      <c r="A21" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1512</v>
+      </c>
+      <c r="C21" s="16">
+        <v>1656</v>
+      </c>
+      <c r="D21" s="16">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="16" customFormat="1">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="12">
+        <f>C20-B20</f>
+        <v>577</v>
+      </c>
+      <c r="D24" s="12">
+        <f>D20-C20</f>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="13">
+        <f>(C20-B20)/B20</f>
+        <v>6.867412520828374E-2</v>
+      </c>
+      <c r="D25" s="13">
+        <f>(D20-C20)/C20</f>
+        <v>5.4905891524668668E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="16" customFormat="1">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" s="16" customFormat="1">
+      <c r="A27" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C27" s="16">
+        <v>337</v>
+      </c>
+      <c r="D27" s="16">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="16" customFormat="1">
+      <c r="A28" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17">
+        <v>0.06</v>
+      </c>
+      <c r="D28" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="1:5" s="16" customFormat="1">
+      <c r="A29" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="16">
+        <v>242</v>
+      </c>
+      <c r="D29" s="16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="16" customFormat="1">
+      <c r="A30" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="D30" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" s="16" customFormat="1">
+      <c r="A31" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C31" s="16">
+        <v>-38</v>
+      </c>
+      <c r="D31" s="16">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="16" customFormat="1">
+      <c r="A32" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17">
+        <v>-0.05</v>
+      </c>
+      <c r="D32" s="17">
+        <v>-0.01</v>
+      </c>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="1:5" s="16" customFormat="1">
+      <c r="A33" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C33" s="16">
+        <v>36</v>
+      </c>
+      <c r="D33" s="16">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="16" customFormat="1">
+      <c r="A34" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="D34" s="17">
+        <v>-0.08</v>
+      </c>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>268</v>
+      </c>
+      <c r="B36" s="10">
+        <v>7253</v>
+      </c>
+      <c r="C36" s="10">
+        <v>8476</v>
+      </c>
+      <c r="D36" s="10">
+        <v>7754</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="10">
+        <v>1202</v>
+      </c>
+      <c r="C37" s="10">
+        <v>1684</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="12">
+        <f>C36-B36</f>
+        <v>1223</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D36-C36</f>
+        <v>-722</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="13">
+        <f>(C36-B36)/B36</f>
+        <v>0.16861988142837447</v>
+      </c>
+      <c r="D41" s="13">
+        <f>(D36-C36)/C36</f>
+        <v>-8.5181689476167999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43">
+        <v>776</v>
+      </c>
+      <c r="D43" s="16">
+        <v>-557</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="17">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16">
+        <v>101</v>
+      </c>
+      <c r="D45" s="16">
+        <v>-233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17">
+        <v>0.06</v>
+      </c>
+      <c r="D46" s="17">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16">
+        <v>140</v>
+      </c>
+      <c r="D47" s="16">
+        <v>-338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="D48" s="17">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16">
+        <v>206</v>
+      </c>
+      <c r="D49" s="16">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="D50" s="17">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="3" customFormat="1">
+      <c r="B55" s="3">
+        <f>B3</f>
+        <v>2021</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" ref="C55:E55" si="1">C3</f>
+        <v>2022</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="1"/>
+        <v>2023</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="1"/>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>256</v>
+      </c>
+      <c r="E57">
+        <f>+AVERAGE(17.4,17.7)</f>
+        <v>17.549999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
         <v>249</v>
       </c>
-      <c r="C19" s="18">
-        <v>-0.01</v>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2228,6 +2870,9 @@
     <hyperlink ref="A1" location="main!A1" display="main" xr:uid="{51A5440C-8489-4FAA-B8B2-3F3E7C0A06BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>